<commit_message>
Working code for FTCS and Lax-Friedrichs. Errors with exact solutuion for CFL != 1
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -1045,7 +1045,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0</v>
+        <v>-0.125</v>
       </c>
       <c r="B3" t="n">
         <v>0</v>
@@ -1081,7 +1081,7 @@
         <v>2.5</v>
       </c>
       <c r="M3" t="n">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="N3" t="n">
         <v>3</v>
@@ -1117,7 +1117,7 @@
         <v>0.5</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="Z3" t="n">
         <v>0</v>
@@ -1350,10 +1350,10 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0</v>
+        <v>-0.125</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>-0.1875</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -1383,13 +1383,13 @@
         <v>2</v>
       </c>
       <c r="L4" t="n">
-        <v>2.25</v>
+        <v>2.125</v>
       </c>
       <c r="M4" t="n">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="N4" t="n">
-        <v>2.75</v>
+        <v>3.125</v>
       </c>
       <c r="O4" t="n">
         <v>3</v>
@@ -1419,13 +1419,13 @@
         <v>1</v>
       </c>
       <c r="X4" t="n">
-        <v>0.75</v>
+        <v>0.8125</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.5</v>
+        <v>0.375</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.25</v>
+        <v>0.0625</v>
       </c>
       <c r="AA4" t="n">
         <v>0</v>
@@ -1655,13 +1655,13 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0</v>
+        <v>-0.03125</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>-0.21875</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -1685,19 +1685,19 @@
         <v>1.5</v>
       </c>
       <c r="K5" t="n">
+        <v>1.8125</v>
+      </c>
+      <c r="L5" t="n">
         <v>1.75</v>
-      </c>
-      <c r="L5" t="n">
-        <v>2</v>
       </c>
       <c r="M5" t="n">
         <v>2.25</v>
       </c>
       <c r="N5" t="n">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="O5" t="n">
-        <v>2.75</v>
+        <v>3.1875</v>
       </c>
       <c r="P5" t="n">
         <v>3</v>
@@ -1721,19 +1721,19 @@
         <v>1.5</v>
       </c>
       <c r="W5" t="n">
-        <v>1.25</v>
+        <v>1.21875</v>
       </c>
       <c r="X5" t="n">
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="Y5" t="n">
         <v>0.75</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.25</v>
+        <v>0.03125</v>
       </c>
       <c r="AB5" t="n">
         <v>0</v>
@@ -1960,16 +1960,16 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0</v>
+        <v>0.09375</v>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>-0.15625</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>-0.34375</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>-0.234375</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -1987,25 +1987,25 @@
         <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>1.25</v>
+        <v>1.21875</v>
       </c>
       <c r="K6" t="n">
-        <v>1.5</v>
+        <v>1.6875</v>
       </c>
       <c r="L6" t="n">
-        <v>1.75</v>
+        <v>1.53125</v>
       </c>
       <c r="M6" t="n">
-        <v>2</v>
+        <v>1.625</v>
       </c>
       <c r="N6" t="n">
-        <v>2.25</v>
+        <v>2.53125</v>
       </c>
       <c r="O6" t="n">
-        <v>2.5</v>
+        <v>3.1875</v>
       </c>
       <c r="P6" t="n">
-        <v>2.75</v>
+        <v>3.21875</v>
       </c>
       <c r="Q6" t="n">
         <v>3</v>
@@ -2023,25 +2023,25 @@
         <v>2</v>
       </c>
       <c r="V6" t="n">
-        <v>1.75</v>
+        <v>1.765625</v>
       </c>
       <c r="W6" t="n">
-        <v>1.5</v>
+        <v>1.40625</v>
       </c>
       <c r="X6" t="n">
-        <v>1.25</v>
+        <v>1.359375</v>
       </c>
       <c r="Y6" t="n">
-        <v>1</v>
+        <v>1.1875</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.75</v>
+        <v>0.609375</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.5</v>
+        <v>0.15625</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.25</v>
+        <v>0.015625</v>
       </c>
       <c r="AC6" t="n">
         <v>0</v>
@@ -2265,19 +2265,19 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0</v>
+        <v>0.171875</v>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>0.0625</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>-0.3046875</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>-0.40625</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>-0.2421875</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -2289,31 +2289,31 @@
         <v>0.5</v>
       </c>
       <c r="I7" t="n">
-        <v>0.75</v>
+        <v>0.765625</v>
       </c>
       <c r="J7" t="n">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="K7" t="n">
-        <v>1.25</v>
+        <v>1.53125</v>
       </c>
       <c r="L7" t="n">
-        <v>1.5</v>
+        <v>1.5625</v>
       </c>
       <c r="M7" t="n">
+        <v>1.125</v>
+      </c>
+      <c r="N7" t="n">
         <v>1.75</v>
       </c>
-      <c r="N7" t="n">
-        <v>2</v>
-      </c>
       <c r="O7" t="n">
-        <v>2.25</v>
+        <v>2.84375</v>
       </c>
       <c r="P7" t="n">
-        <v>2.5</v>
+        <v>3.3125</v>
       </c>
       <c r="Q7" t="n">
-        <v>2.75</v>
+        <v>3.234375</v>
       </c>
       <c r="R7" t="n">
         <v>3</v>
@@ -2325,31 +2325,31 @@
         <v>2.5</v>
       </c>
       <c r="U7" t="n">
-        <v>2.25</v>
+        <v>2.2421875</v>
       </c>
       <c r="V7" t="n">
-        <v>2</v>
+        <v>2.0625</v>
       </c>
       <c r="W7" t="n">
-        <v>1.75</v>
+        <v>1.609375</v>
       </c>
       <c r="X7" t="n">
-        <v>1.5</v>
+        <v>1.46875</v>
       </c>
       <c r="Y7" t="n">
-        <v>1.25</v>
+        <v>1.5625</v>
       </c>
       <c r="Z7" t="n">
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.75</v>
+        <v>0.453125</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.5</v>
+        <v>0.09375</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.25</v>
+        <v>0.0078125</v>
       </c>
       <c r="AD7" t="n">
         <v>0</v>
@@ -2570,94 +2570,94 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0</v>
+        <v>0.140625</v>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>0.30078125</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>-0.0703125</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>-0.4375</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>-0.4453125</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>-0.24609375</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>0.25</v>
+        <v>0.2421875</v>
       </c>
       <c r="I8" t="n">
-        <v>0.5</v>
+        <v>0.578125</v>
       </c>
       <c r="J8" t="n">
-        <v>0.75</v>
+        <v>0.4921875</v>
       </c>
       <c r="K8" t="n">
-        <v>1</v>
+        <v>1.1875</v>
       </c>
       <c r="L8" t="n">
-        <v>1.25</v>
+        <v>1.765625</v>
       </c>
       <c r="M8" t="n">
-        <v>1.5</v>
+        <v>1.03125</v>
       </c>
       <c r="N8" t="n">
-        <v>1.75</v>
+        <v>0.890625</v>
       </c>
       <c r="O8" t="n">
-        <v>2</v>
+        <v>2.0625</v>
       </c>
       <c r="P8" t="n">
-        <v>2.25</v>
+        <v>3.1171875</v>
       </c>
       <c r="Q8" t="n">
-        <v>2.5</v>
+        <v>3.390625</v>
       </c>
       <c r="R8" t="n">
-        <v>2.75</v>
+        <v>3.2421875</v>
       </c>
       <c r="S8" t="n">
         <v>3</v>
       </c>
       <c r="T8" t="n">
-        <v>2.75</v>
+        <v>2.75390625</v>
       </c>
       <c r="U8" t="n">
-        <v>2.5</v>
+        <v>2.4609375</v>
       </c>
       <c r="V8" t="n">
-        <v>2.25</v>
+        <v>2.37890625</v>
       </c>
       <c r="W8" t="n">
-        <v>2</v>
+        <v>1.90625</v>
       </c>
       <c r="X8" t="n">
-        <v>1.75</v>
+        <v>1.4921875</v>
       </c>
       <c r="Y8" t="n">
-        <v>1.5</v>
+        <v>1.734375</v>
       </c>
       <c r="Z8" t="n">
-        <v>1.25</v>
+        <v>1.6796875</v>
       </c>
       <c r="AA8" t="n">
-        <v>1</v>
+        <v>0.96875</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.75</v>
+        <v>0.31640625</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.5</v>
+        <v>0.0546875</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.25</v>
+        <v>0.00390625</v>
       </c>
       <c r="AE8" t="n">
         <v>0</v>
@@ -2875,97 +2875,97 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0</v>
+        <v>-0.009765625</v>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>0.40625</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>0.298828125</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>-0.541015625</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>-0.46875</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>-0.244140625</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>-0.046875</v>
       </c>
       <c r="I9" t="n">
-        <v>0.25</v>
+        <v>0.453125</v>
       </c>
       <c r="J9" t="n">
-        <v>0.5</v>
+        <v>0.1875</v>
       </c>
       <c r="K9" t="n">
-        <v>0.75</v>
+        <v>0.55078125</v>
       </c>
       <c r="L9" t="n">
-        <v>1</v>
+        <v>1.84375</v>
       </c>
       <c r="M9" t="n">
-        <v>1.25</v>
+        <v>1.46875</v>
       </c>
       <c r="N9" t="n">
-        <v>1.5</v>
+        <v>0.375</v>
       </c>
       <c r="O9" t="n">
-        <v>1.75</v>
+        <v>0.94921875</v>
       </c>
       <c r="P9" t="n">
-        <v>2</v>
+        <v>2.453125</v>
       </c>
       <c r="Q9" t="n">
-        <v>2.25</v>
+        <v>3.328125</v>
       </c>
       <c r="R9" t="n">
-        <v>2.5</v>
+        <v>3.4375</v>
       </c>
       <c r="S9" t="n">
-        <v>2.75</v>
+        <v>3.244140625</v>
       </c>
       <c r="T9" t="n">
-        <v>3</v>
+        <v>3.0234375</v>
       </c>
       <c r="U9" t="n">
-        <v>2.75</v>
+        <v>2.6484375</v>
       </c>
       <c r="V9" t="n">
-        <v>2.5</v>
+        <v>2.65625</v>
       </c>
       <c r="W9" t="n">
-        <v>2.25</v>
+        <v>2.349609375</v>
       </c>
       <c r="X9" t="n">
-        <v>2</v>
+        <v>1.578125</v>
       </c>
       <c r="Y9" t="n">
-        <v>1.75</v>
+        <v>1.640625</v>
       </c>
       <c r="Z9" t="n">
-        <v>1.5</v>
+        <v>2.0625</v>
       </c>
       <c r="AA9" t="n">
-        <v>1.25</v>
+        <v>1.650390625</v>
       </c>
       <c r="AB9" t="n">
-        <v>1</v>
+        <v>0.7734375</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.75</v>
+        <v>0.2109375</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.5</v>
+        <v>0.03125</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.25</v>
+        <v>0.001953125</v>
       </c>
       <c r="AF9" t="n">
         <v>0</v>
@@ -3180,100 +3180,100 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0</v>
+        <v>-0.212890625</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>0.251953125</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>0.626953125</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>0.169921875</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>-0.431640625</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>-0.6171875</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>-0.455078125</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>-0.3955078125</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>0.3359375</v>
       </c>
       <c r="J10" t="n">
-        <v>0.25</v>
+        <v>0.138671875</v>
       </c>
       <c r="K10" t="n">
-        <v>0.5</v>
+        <v>-0.27734375</v>
       </c>
       <c r="L10" t="n">
-        <v>0.75</v>
+        <v>1.384765625</v>
       </c>
       <c r="M10" t="n">
-        <v>1</v>
+        <v>2.203125</v>
       </c>
       <c r="N10" t="n">
-        <v>1.25</v>
+        <v>0.634765625</v>
       </c>
       <c r="O10" t="n">
-        <v>1.5</v>
+        <v>-0.08984375</v>
       </c>
       <c r="P10" t="n">
-        <v>1.75</v>
+        <v>1.263671875</v>
       </c>
       <c r="Q10" t="n">
-        <v>2</v>
+        <v>2.8359375</v>
       </c>
       <c r="R10" t="n">
-        <v>2.25</v>
+        <v>3.4794921875</v>
       </c>
       <c r="S10" t="n">
-        <v>2.5</v>
+        <v>3.451171875</v>
       </c>
       <c r="T10" t="n">
-        <v>2.75</v>
+        <v>3.3212890625</v>
       </c>
       <c r="U10" t="n">
-        <v>3</v>
+        <v>2.83203125</v>
       </c>
       <c r="V10" t="n">
-        <v>2.75</v>
+        <v>2.8056640625</v>
       </c>
       <c r="W10" t="n">
-        <v>2.5</v>
+        <v>2.888671875</v>
       </c>
       <c r="X10" t="n">
-        <v>2.25</v>
+        <v>1.9326171875</v>
       </c>
       <c r="Y10" t="n">
-        <v>2</v>
+        <v>1.3984375</v>
       </c>
       <c r="Z10" t="n">
-        <v>1.75</v>
+        <v>2.0576171875</v>
       </c>
       <c r="AA10" t="n">
-        <v>1.5</v>
+        <v>2.294921875</v>
       </c>
       <c r="AB10" t="n">
-        <v>1.25</v>
+        <v>1.4931640625</v>
       </c>
       <c r="AC10" t="n">
-        <v>1</v>
+        <v>0.58203125</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.75</v>
+        <v>0.1357421875</v>
       </c>
       <c r="AE10" t="n">
-        <v>0.5</v>
+        <v>0.017578125</v>
       </c>
       <c r="AF10" t="n">
-        <v>0.25</v>
+        <v>0.0009765625</v>
       </c>
       <c r="AG10" t="n">
         <v>0</v>
@@ -3485,103 +3485,103 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0</v>
+        <v>-0.3388671875</v>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>-0.16796875</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>0.66796875</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>0.69921875</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>-0.0380859375</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>-0.60546875</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>-0.56591796875</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>-0.791015625</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>0.06884765625</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>0.4453125</v>
       </c>
       <c r="K11" t="n">
-        <v>0.25</v>
+        <v>-0.900390625</v>
       </c>
       <c r="L11" t="n">
-        <v>0.5</v>
+        <v>0.14453125</v>
       </c>
       <c r="M11" t="n">
-        <v>0.75</v>
+        <v>2.578125</v>
       </c>
       <c r="N11" t="n">
-        <v>1</v>
+        <v>1.78125</v>
       </c>
       <c r="O11" t="n">
-        <v>1.25</v>
+        <v>-0.404296875</v>
       </c>
       <c r="P11" t="n">
-        <v>1.5</v>
+        <v>-0.19921875</v>
       </c>
       <c r="Q11" t="n">
-        <v>1.75</v>
+        <v>1.72802734375</v>
       </c>
       <c r="R11" t="n">
-        <v>2</v>
+        <v>3.171875</v>
       </c>
       <c r="S11" t="n">
-        <v>2.25</v>
+        <v>3.5302734375</v>
       </c>
       <c r="T11" t="n">
-        <v>2.5</v>
+        <v>3.630859375</v>
       </c>
       <c r="U11" t="n">
-        <v>2.75</v>
+        <v>3.08984375</v>
       </c>
       <c r="V11" t="n">
-        <v>3</v>
+        <v>2.77734375</v>
       </c>
       <c r="W11" t="n">
-        <v>2.75</v>
+        <v>3.3251953125</v>
       </c>
       <c r="X11" t="n">
-        <v>2.5</v>
+        <v>2.677734375</v>
       </c>
       <c r="Y11" t="n">
-        <v>2.25</v>
+        <v>1.3359375</v>
       </c>
       <c r="Z11" t="n">
-        <v>2</v>
+        <v>1.609375</v>
       </c>
       <c r="AA11" t="n">
-        <v>1.75</v>
+        <v>2.5771484375</v>
       </c>
       <c r="AB11" t="n">
-        <v>1.5</v>
+        <v>2.349609375</v>
       </c>
       <c r="AC11" t="n">
-        <v>1.25</v>
+        <v>1.2607421875</v>
       </c>
       <c r="AD11" t="n">
-        <v>1</v>
+        <v>0.41796875</v>
       </c>
       <c r="AE11" t="n">
-        <v>0.75</v>
+        <v>0.0849609375</v>
       </c>
       <c r="AF11" t="n">
-        <v>0.5</v>
+        <v>0.009765625</v>
       </c>
       <c r="AG11" t="n">
-        <v>0.25</v>
+        <v>0.00048828125</v>
       </c>
       <c r="AH11" t="n">
         <v>0</v>
@@ -3790,106 +3790,106 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0</v>
+        <v>-0.2548828125</v>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>-0.67138671875</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>0.234375</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>1.05224609375</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>0.6142578125</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>-0.341552734375</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>-0.47314453125</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>-1.1083984375</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>-0.54931640625</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>0.929931640625</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>-0.75</v>
       </c>
       <c r="L12" t="n">
-        <v>0.25</v>
+        <v>-1.5947265625</v>
       </c>
       <c r="M12" t="n">
-        <v>0.5</v>
+        <v>1.759765625</v>
       </c>
       <c r="N12" t="n">
-        <v>0.75</v>
+        <v>3.2724609375</v>
       </c>
       <c r="O12" t="n">
-        <v>1</v>
+        <v>0.5859375</v>
       </c>
       <c r="P12" t="n">
-        <v>1.25</v>
+        <v>-1.265380859375</v>
       </c>
       <c r="Q12" t="n">
-        <v>1.5</v>
+        <v>0.04248046875</v>
       </c>
       <c r="R12" t="n">
-        <v>1.75</v>
+        <v>2.270751953125</v>
       </c>
       <c r="S12" t="n">
-        <v>2</v>
+        <v>3.30078125</v>
       </c>
       <c r="T12" t="n">
-        <v>2.25</v>
+        <v>3.85107421875</v>
       </c>
       <c r="U12" t="n">
-        <v>2.5</v>
+        <v>3.5166015625</v>
       </c>
       <c r="V12" t="n">
-        <v>2.75</v>
+        <v>2.65966796875</v>
       </c>
       <c r="W12" t="n">
-        <v>3</v>
+        <v>3.375</v>
       </c>
       <c r="X12" t="n">
-        <v>2.75</v>
+        <v>3.67236328125</v>
       </c>
       <c r="Y12" t="n">
-        <v>2.5</v>
+        <v>1.8701171875</v>
       </c>
       <c r="Z12" t="n">
-        <v>2.25</v>
+        <v>0.98876953125</v>
       </c>
       <c r="AA12" t="n">
-        <v>2</v>
+        <v>2.20703125</v>
       </c>
       <c r="AB12" t="n">
-        <v>1.75</v>
+        <v>3.0078125</v>
       </c>
       <c r="AC12" t="n">
-        <v>1.5</v>
+        <v>2.2265625</v>
       </c>
       <c r="AD12" t="n">
-        <v>1.25</v>
+        <v>1.005859375</v>
       </c>
       <c r="AE12" t="n">
-        <v>1</v>
+        <v>0.2890625</v>
       </c>
       <c r="AF12" t="n">
-        <v>0.75</v>
+        <v>0.052001953125</v>
       </c>
       <c r="AG12" t="n">
-        <v>0.5</v>
+        <v>0.00537109375</v>
       </c>
       <c r="AH12" t="n">
-        <v>0.25</v>
+        <v>0.000244140625</v>
       </c>
       <c r="AI12" t="n">
         <v>0</v>
@@ -4095,109 +4095,109 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0</v>
+        <v>0.080810546875</v>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>-0.916015625</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>-0.62744140625</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>0.8623046875</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>1.3111572265625</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>0.2021484375</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>-0.0897216796875</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>-1.0703125</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>-1.5684814453125</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>1.0302734375</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>0.5123291015625</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>-2.849609375</v>
       </c>
       <c r="M13" t="n">
-        <v>0.25</v>
+        <v>-0.673828125</v>
       </c>
       <c r="N13" t="n">
-        <v>0.5</v>
+        <v>3.859375</v>
       </c>
       <c r="O13" t="n">
-        <v>0.75</v>
+        <v>2.8548583984375</v>
       </c>
       <c r="P13" t="n">
-        <v>1</v>
+        <v>-0.99365234375</v>
       </c>
       <c r="Q13" t="n">
-        <v>1.25</v>
+        <v>-1.7255859375</v>
       </c>
       <c r="R13" t="n">
-        <v>1.5</v>
+        <v>0.6416015625</v>
       </c>
       <c r="S13" t="n">
-        <v>1.75</v>
+        <v>2.5106201171875</v>
       </c>
       <c r="T13" t="n">
-        <v>2</v>
+        <v>3.7431640625</v>
       </c>
       <c r="U13" t="n">
-        <v>2.25</v>
+        <v>4.1123046875</v>
       </c>
       <c r="V13" t="n">
-        <v>2.5</v>
+        <v>2.73046875</v>
       </c>
       <c r="W13" t="n">
-        <v>2.75</v>
+        <v>2.86865234375</v>
       </c>
       <c r="X13" t="n">
-        <v>3</v>
+        <v>4.4248046875</v>
       </c>
       <c r="Y13" t="n">
-        <v>2.75</v>
+        <v>3.2119140625</v>
       </c>
       <c r="Z13" t="n">
-        <v>2.5</v>
+        <v>0.8203125</v>
       </c>
       <c r="AA13" t="n">
-        <v>2.25</v>
+        <v>1.197509765625</v>
       </c>
       <c r="AB13" t="n">
-        <v>2</v>
+        <v>2.998046875</v>
       </c>
       <c r="AC13" t="n">
-        <v>1.75</v>
+        <v>3.2275390625</v>
       </c>
       <c r="AD13" t="n">
-        <v>1.5</v>
+        <v>1.974609375</v>
       </c>
       <c r="AE13" t="n">
-        <v>1.25</v>
+        <v>0.7659912109375</v>
       </c>
       <c r="AF13" t="n">
-        <v>1</v>
+        <v>0.19384765625</v>
       </c>
       <c r="AG13" t="n">
-        <v>0.75</v>
+        <v>0.03125</v>
       </c>
       <c r="AH13" t="n">
-        <v>0.5</v>
+        <v>0.0029296875</v>
       </c>
       <c r="AI13" t="n">
-        <v>0.25</v>
+        <v>0.0001220703125</v>
       </c>
       <c r="AJ13" t="n">
         <v>0</v>
@@ -4400,112 +4400,112 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0</v>
+        <v>0.538818359375</v>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>-0.5618896484375</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>-1.5166015625</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>-0.10699462890625</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>1.6412353515625</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>0.902587890625</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>0.5465087890625</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>-0.3309326171875</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>-2.6187744140625</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>-0.0101318359375</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>2.4522705078125</v>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
+        <v>-2.25653076171875</v>
       </c>
       <c r="M14" t="n">
-        <v>0</v>
+        <v>-4.0283203125</v>
       </c>
       <c r="N14" t="n">
-        <v>0.25</v>
+        <v>2.09503173828125</v>
       </c>
       <c r="O14" t="n">
-        <v>0.5</v>
+        <v>5.2813720703125</v>
       </c>
       <c r="P14" t="n">
-        <v>0.75</v>
+        <v>1.29656982421875</v>
       </c>
       <c r="Q14" t="n">
-        <v>1</v>
+        <v>-2.543212890625</v>
       </c>
       <c r="R14" t="n">
-        <v>1.25</v>
+        <v>-1.47650146484375</v>
       </c>
       <c r="S14" t="n">
-        <v>1.5</v>
+        <v>0.9598388671875</v>
       </c>
       <c r="T14" t="n">
-        <v>1.75</v>
+        <v>2.94232177734375</v>
       </c>
       <c r="U14" t="n">
-        <v>2</v>
+        <v>4.61865234375</v>
       </c>
       <c r="V14" t="n">
-        <v>2.25</v>
+        <v>3.352294921875</v>
       </c>
       <c r="W14" t="n">
-        <v>2.5</v>
+        <v>2.021484375</v>
       </c>
       <c r="X14" t="n">
-        <v>2.75</v>
+        <v>4.253173828125</v>
       </c>
       <c r="Y14" t="n">
-        <v>3</v>
+        <v>5.01416015625</v>
       </c>
       <c r="Z14" t="n">
-        <v>2.75</v>
+        <v>1.8275146484375</v>
       </c>
       <c r="AA14" t="n">
-        <v>2.5</v>
+        <v>0.108642578125</v>
       </c>
       <c r="AB14" t="n">
-        <v>2.25</v>
+        <v>1.9830322265625</v>
       </c>
       <c r="AC14" t="n">
-        <v>2</v>
+        <v>3.7392578125</v>
       </c>
       <c r="AD14" t="n">
-        <v>1.75</v>
+        <v>3.20538330078125</v>
       </c>
       <c r="AE14" t="n">
-        <v>1.5</v>
+        <v>1.6563720703125</v>
       </c>
       <c r="AF14" t="n">
-        <v>1.25</v>
+        <v>0.56121826171875</v>
       </c>
       <c r="AG14" t="n">
-        <v>1</v>
+        <v>0.126708984375</v>
       </c>
       <c r="AH14" t="n">
-        <v>0.75</v>
+        <v>0.01849365234375</v>
       </c>
       <c r="AI14" t="n">
-        <v>0.5</v>
+        <v>0.0015869140625</v>
       </c>
       <c r="AJ14" t="n">
-        <v>0.25</v>
+        <v>6.103515625e-05</v>
       </c>
       <c r="AK14" t="n">
         <v>0</v>
@@ -4705,115 +4705,115 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0</v>
+        <v>0.81976318359375</v>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>0.4658203125</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>-1.744049072265625</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>-1.6859130859375</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>1.136444091796875</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>1.449951171875</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>1.16326904296875</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>1.251708984375</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>-2.7791748046875</v>
       </c>
       <c r="J15" t="n">
-        <v>0</v>
+        <v>-2.545654296875</v>
       </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>3.575469970703125</v>
       </c>
       <c r="L15" t="n">
-        <v>0</v>
+        <v>0.9837646484375</v>
       </c>
       <c r="M15" t="n">
-        <v>0</v>
+        <v>-6.2041015625</v>
       </c>
       <c r="N15" t="n">
-        <v>0</v>
+        <v>-2.559814453125</v>
       </c>
       <c r="O15" t="n">
-        <v>0.25</v>
+        <v>5.68060302734375</v>
       </c>
       <c r="P15" t="n">
-        <v>0.5</v>
+        <v>5.2088623046875</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.75</v>
+        <v>-1.15667724609375</v>
       </c>
       <c r="R15" t="n">
-        <v>1</v>
+        <v>-3.22802734375</v>
       </c>
       <c r="S15" t="n">
-        <v>1.25</v>
+        <v>-1.24957275390625</v>
       </c>
       <c r="T15" t="n">
-        <v>1.5</v>
+        <v>1.1129150390625</v>
       </c>
       <c r="U15" t="n">
-        <v>1.75</v>
+        <v>4.413665771484375</v>
       </c>
       <c r="V15" t="n">
-        <v>2</v>
+        <v>4.65087890625</v>
       </c>
       <c r="W15" t="n">
-        <v>2.25</v>
+        <v>1.571044921875</v>
       </c>
       <c r="X15" t="n">
-        <v>2.5</v>
+        <v>2.7568359375</v>
       </c>
       <c r="Y15" t="n">
-        <v>2.75</v>
+        <v>6.22698974609375</v>
       </c>
       <c r="Z15" t="n">
-        <v>3</v>
+        <v>4.2802734375</v>
       </c>
       <c r="AA15" t="n">
-        <v>2.75</v>
+        <v>0.0308837890625</v>
       </c>
       <c r="AB15" t="n">
-        <v>2.5</v>
+        <v>0.167724609375</v>
       </c>
       <c r="AC15" t="n">
-        <v>2.25</v>
+        <v>3.128082275390625</v>
       </c>
       <c r="AD15" t="n">
-        <v>2</v>
+        <v>4.246826171875</v>
       </c>
       <c r="AE15" t="n">
-        <v>1.75</v>
+        <v>2.97845458984375</v>
       </c>
       <c r="AF15" t="n">
-        <v>1.5</v>
+        <v>1.3260498046875</v>
       </c>
       <c r="AG15" t="n">
-        <v>1.25</v>
+        <v>0.3980712890625</v>
       </c>
       <c r="AH15" t="n">
-        <v>1</v>
+        <v>0.0810546875</v>
       </c>
       <c r="AI15" t="n">
-        <v>0.75</v>
+        <v>0.01080322265625</v>
       </c>
       <c r="AJ15" t="n">
-        <v>0.5</v>
+        <v>0.0008544921875</v>
       </c>
       <c r="AK15" t="n">
-        <v>0.25</v>
+        <v>3.0517578125e-05</v>
       </c>
       <c r="AL15" t="n">
         <v>0</v>
@@ -5010,118 +5010,118 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0</v>
+        <v>0.58685302734375</v>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>1.747726440429688</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>-0.668182373046875</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>-3.12615966796875</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>-0.431488037109375</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>1.436538696289062</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>1.26239013671875</v>
       </c>
       <c r="H16" t="n">
-        <v>0</v>
+        <v>3.222930908203125</v>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>-0.8804931640625</v>
       </c>
       <c r="J16" t="n">
-        <v>0</v>
+        <v>-5.722976684570312</v>
       </c>
       <c r="K16" t="n">
-        <v>0</v>
+        <v>1.810760498046875</v>
       </c>
       <c r="L16" t="n">
-        <v>0</v>
+        <v>5.873550415039062</v>
       </c>
       <c r="M16" t="n">
-        <v>0</v>
+        <v>-4.43231201171875</v>
       </c>
       <c r="N16" t="n">
-        <v>0</v>
+        <v>-8.502166748046875</v>
       </c>
       <c r="O16" t="n">
-        <v>0</v>
+        <v>1.7962646484375</v>
       </c>
       <c r="P16" t="n">
-        <v>0.25</v>
+        <v>8.62750244140625</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.5</v>
+        <v>3.061767578125</v>
       </c>
       <c r="R16" t="n">
-        <v>0.75</v>
+        <v>-3.18157958984375</v>
       </c>
       <c r="S16" t="n">
-        <v>1</v>
+        <v>-3.4200439453125</v>
       </c>
       <c r="T16" t="n">
-        <v>1.25</v>
+        <v>-1.718704223632812</v>
       </c>
       <c r="U16" t="n">
-        <v>1.5</v>
+        <v>2.644683837890625</v>
       </c>
       <c r="V16" t="n">
-        <v>1.75</v>
+        <v>6.072189331054688</v>
       </c>
       <c r="W16" t="n">
-        <v>2</v>
+        <v>2.51806640625</v>
       </c>
       <c r="X16" t="n">
-        <v>2.25</v>
+        <v>0.428863525390625</v>
       </c>
       <c r="Y16" t="n">
-        <v>2.5</v>
+        <v>5.46527099609375</v>
       </c>
       <c r="Z16" t="n">
-        <v>2.75</v>
+        <v>7.378326416015625</v>
       </c>
       <c r="AA16" t="n">
-        <v>3</v>
+        <v>2.087158203125</v>
       </c>
       <c r="AB16" t="n">
-        <v>2.75</v>
+        <v>-1.380874633789062</v>
       </c>
       <c r="AC16" t="n">
-        <v>2.5</v>
+        <v>1.088531494140625</v>
       </c>
       <c r="AD16" t="n">
-        <v>2.25</v>
+        <v>4.321640014648438</v>
       </c>
       <c r="AE16" t="n">
-        <v>2</v>
+        <v>4.4388427734375</v>
       </c>
       <c r="AF16" t="n">
-        <v>1.75</v>
+        <v>2.616241455078125</v>
       </c>
       <c r="AG16" t="n">
-        <v>1.5</v>
+        <v>1.02056884765625</v>
       </c>
       <c r="AH16" t="n">
-        <v>1.25</v>
+        <v>0.274688720703125</v>
       </c>
       <c r="AI16" t="n">
-        <v>1</v>
+        <v>0.0509033203125</v>
       </c>
       <c r="AJ16" t="n">
-        <v>0.75</v>
+        <v>0.0062408447265625</v>
       </c>
       <c r="AK16" t="n">
-        <v>0.5</v>
+        <v>0.000457763671875</v>
       </c>
       <c r="AL16" t="n">
-        <v>0.25</v>
+        <v>1.52587890625e-05</v>
       </c>
       <c r="AM16" t="n">
         <v>0</v>
@@ -5315,121 +5315,121 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0</v>
+        <v>-0.2870101928710938</v>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>2.375244140625</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>1.768760681152344</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>-3.2445068359375</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>-2.712837219238281</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>0.589599609375</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>0.3691940307617188</v>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
+        <v>4.29437255859375</v>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>3.592460632324219</v>
       </c>
       <c r="J17" t="n">
-        <v>0</v>
+        <v>-7.068603515625</v>
       </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>-3.987503051757812</v>
       </c>
       <c r="L17" t="n">
-        <v>0</v>
+        <v>8.995086669921875</v>
       </c>
       <c r="M17" t="n">
-        <v>0</v>
+        <v>2.755546569824219</v>
       </c>
       <c r="N17" t="n">
-        <v>0</v>
+        <v>-11.616455078125</v>
       </c>
       <c r="O17" t="n">
-        <v>0</v>
+        <v>-6.768569946289062</v>
       </c>
       <c r="P17" t="n">
-        <v>0</v>
+        <v>7.9947509765625</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.25</v>
+        <v>8.96630859375</v>
       </c>
       <c r="R17" t="n">
-        <v>0.5</v>
+        <v>0.059326171875</v>
       </c>
       <c r="S17" t="n">
-        <v>0.75</v>
+        <v>-4.151481628417969</v>
       </c>
       <c r="T17" t="n">
-        <v>1</v>
+        <v>-4.751068115234375</v>
       </c>
       <c r="U17" t="n">
-        <v>1.25</v>
+        <v>-1.250762939453125</v>
       </c>
       <c r="V17" t="n">
-        <v>1.5</v>
+        <v>6.135498046875</v>
       </c>
       <c r="W17" t="n">
-        <v>1.75</v>
+        <v>5.339729309082031</v>
       </c>
       <c r="X17" t="n">
-        <v>2</v>
+        <v>-1.04473876953125</v>
       </c>
       <c r="Y17" t="n">
-        <v>2.25</v>
+        <v>1.99053955078125</v>
       </c>
       <c r="Z17" t="n">
-        <v>2.5</v>
+        <v>9.0673828125</v>
       </c>
       <c r="AA17" t="n">
-        <v>2.75</v>
+        <v>6.466758728027344</v>
       </c>
       <c r="AB17" t="n">
-        <v>3</v>
+        <v>-0.881561279296875</v>
       </c>
       <c r="AC17" t="n">
-        <v>2.75</v>
+        <v>-1.762725830078125</v>
       </c>
       <c r="AD17" t="n">
-        <v>2.5</v>
+        <v>2.646484375</v>
       </c>
       <c r="AE17" t="n">
-        <v>2.25</v>
+        <v>5.291542053222656</v>
       </c>
       <c r="AF17" t="n">
-        <v>2</v>
+        <v>4.32537841796875</v>
       </c>
       <c r="AG17" t="n">
-        <v>1.75</v>
+        <v>2.19134521484375</v>
       </c>
       <c r="AH17" t="n">
-        <v>1.5</v>
+        <v>0.759521484375</v>
       </c>
       <c r="AI17" t="n">
-        <v>1.25</v>
+        <v>0.1851272583007812</v>
       </c>
       <c r="AJ17" t="n">
-        <v>1</v>
+        <v>0.031463623046875</v>
       </c>
       <c r="AK17" t="n">
-        <v>0.75</v>
+        <v>0.003570556640625</v>
       </c>
       <c r="AL17" t="n">
-        <v>0.5</v>
+        <v>0.000244140625</v>
       </c>
       <c r="AM17" t="n">
-        <v>0.25</v>
+        <v>7.62939453125e-06</v>
       </c>
       <c r="AN17" t="n">
         <v>0</v>
@@ -5620,124 +5620,124 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0</v>
+        <v>-1.474632263183594</v>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>1.347358703613281</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>4.578636169433594</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>-1.003707885742188</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>-4.629890441894531</v>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>-0.951416015625</v>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>-1.483192443847656</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>2.6827392578125</v>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>9.273948669433594</v>
       </c>
       <c r="J18" t="n">
-        <v>0</v>
+        <v>-3.278621673583984</v>
       </c>
       <c r="K18" t="n">
-        <v>0</v>
+        <v>-12.01934814453125</v>
       </c>
       <c r="L18" t="n">
-        <v>0</v>
+        <v>5.623561859130859</v>
       </c>
       <c r="M18" t="n">
-        <v>0</v>
+        <v>13.06131744384766</v>
       </c>
       <c r="N18" t="n">
-        <v>0</v>
+        <v>-6.854396820068359</v>
       </c>
       <c r="O18" t="n">
-        <v>0</v>
+        <v>-16.57417297363281</v>
       </c>
       <c r="P18" t="n">
-        <v>0</v>
+        <v>0.1273117065429688</v>
       </c>
       <c r="Q18" t="n">
-        <v>0</v>
+        <v>12.93402099609375</v>
       </c>
       <c r="R18" t="n">
-        <v>0.25</v>
+        <v>6.618221282958984</v>
       </c>
       <c r="S18" t="n">
-        <v>0.5</v>
+        <v>-1.746284484863281</v>
       </c>
       <c r="T18" t="n">
-        <v>0.75</v>
+        <v>-6.201427459716797</v>
       </c>
       <c r="U18" t="n">
-        <v>1</v>
+        <v>-6.694046020507812</v>
       </c>
       <c r="V18" t="n">
-        <v>1.25</v>
+        <v>2.840251922607422</v>
       </c>
       <c r="W18" t="n">
-        <v>1.5</v>
+        <v>8.929847717285156</v>
       </c>
       <c r="X18" t="n">
-        <v>1.75</v>
+        <v>0.6298561096191406</v>
       </c>
       <c r="Y18" t="n">
-        <v>2</v>
+        <v>-3.065521240234375</v>
       </c>
       <c r="Z18" t="n">
-        <v>2.25</v>
+        <v>6.829273223876953</v>
       </c>
       <c r="AA18" t="n">
-        <v>2.5</v>
+        <v>11.44123077392578</v>
       </c>
       <c r="AB18" t="n">
-        <v>2.75</v>
+        <v>3.233180999755859</v>
       </c>
       <c r="AC18" t="n">
-        <v>3</v>
+        <v>-3.526748657226562</v>
       </c>
       <c r="AD18" t="n">
-        <v>2.75</v>
+        <v>-0.8806495666503906</v>
       </c>
       <c r="AE18" t="n">
-        <v>2.5</v>
+        <v>4.452095031738281</v>
       </c>
       <c r="AF18" t="n">
-        <v>2.25</v>
+        <v>5.875476837158203</v>
       </c>
       <c r="AG18" t="n">
-        <v>2</v>
+        <v>3.974273681640625</v>
       </c>
       <c r="AH18" t="n">
-        <v>1.75</v>
+        <v>1.762630462646484</v>
       </c>
       <c r="AI18" t="n">
-        <v>1.5</v>
+        <v>0.5491561889648438</v>
       </c>
       <c r="AJ18" t="n">
-        <v>1.25</v>
+        <v>0.1222419738769531</v>
       </c>
       <c r="AK18" t="n">
-        <v>1</v>
+        <v>0.0191802978515625</v>
       </c>
       <c r="AL18" t="n">
-        <v>0.75</v>
+        <v>0.002025604248046875</v>
       </c>
       <c r="AM18" t="n">
-        <v>0.5</v>
+        <v>0.00012969970703125</v>
       </c>
       <c r="AN18" t="n">
-        <v>0.25</v>
+        <v>3.814697265625e-06</v>
       </c>
       <c r="AO18" t="n">
         <v>0</v>
@@ -5925,127 +5925,127 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0</v>
+        <v>-2.148311614990234</v>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
+        <v>-1.679275512695312</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>5.754169464111328</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>3.600555419921875</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>-4.656036376953125</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>-2.524765014648438</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>-3.300270080566406</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>-2.695831298828125</v>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>12.25462913513184</v>
       </c>
       <c r="J19" t="n">
-        <v>0</v>
+        <v>7.368026733398438</v>
       </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>-16.47043991088867</v>
       </c>
       <c r="L19" t="n">
-        <v>0</v>
+        <v>-6.916770935058594</v>
       </c>
       <c r="M19" t="n">
-        <v>0</v>
+        <v>19.30029678344727</v>
       </c>
       <c r="N19" t="n">
-        <v>0</v>
+        <v>7.963348388671875</v>
       </c>
       <c r="O19" t="n">
-        <v>0</v>
+        <v>-20.06502723693848</v>
       </c>
       <c r="P19" t="n">
-        <v>0</v>
+        <v>-14.62678527832031</v>
       </c>
       <c r="Q19" t="n">
-        <v>0</v>
+        <v>9.688566207885742</v>
       </c>
       <c r="R19" t="n">
-        <v>0</v>
+        <v>13.9583740234375</v>
       </c>
       <c r="S19" t="n">
-        <v>0.25</v>
+        <v>4.663539886474609</v>
       </c>
       <c r="T19" t="n">
-        <v>0.5</v>
+        <v>-3.727546691894531</v>
       </c>
       <c r="U19" t="n">
-        <v>0.75</v>
+        <v>-11.21488571166992</v>
       </c>
       <c r="V19" t="n">
-        <v>1</v>
+        <v>-4.971694946289062</v>
       </c>
       <c r="W19" t="n">
-        <v>1.25</v>
+        <v>10.0350456237793</v>
       </c>
       <c r="X19" t="n">
-        <v>1.5</v>
+        <v>6.627540588378906</v>
       </c>
       <c r="Y19" t="n">
-        <v>1.75</v>
+        <v>-6.165229797363281</v>
       </c>
       <c r="Z19" t="n">
-        <v>2</v>
+        <v>-0.424102783203125</v>
       </c>
       <c r="AA19" t="n">
-        <v>2.25</v>
+        <v>13.23927688598633</v>
       </c>
       <c r="AB19" t="n">
-        <v>2.5</v>
+        <v>10.71717071533203</v>
       </c>
       <c r="AC19" t="n">
-        <v>2.75</v>
+        <v>-1.469833374023438</v>
       </c>
       <c r="AD19" t="n">
-        <v>3</v>
+        <v>-4.870071411132812</v>
       </c>
       <c r="AE19" t="n">
-        <v>2.75</v>
+        <v>1.074031829833984</v>
       </c>
       <c r="AF19" t="n">
-        <v>2.5</v>
+        <v>6.114387512207031</v>
       </c>
       <c r="AG19" t="n">
-        <v>2.25</v>
+        <v>6.030696868896484</v>
       </c>
       <c r="AH19" t="n">
-        <v>2</v>
+        <v>3.475189208984375</v>
       </c>
       <c r="AI19" t="n">
-        <v>1.75</v>
+        <v>1.369350433349609</v>
       </c>
       <c r="AJ19" t="n">
-        <v>1.5</v>
+        <v>0.3872299194335938</v>
       </c>
       <c r="AK19" t="n">
-        <v>1.25</v>
+        <v>0.07928848266601562</v>
       </c>
       <c r="AL19" t="n">
-        <v>1</v>
+        <v>0.0115509033203125</v>
       </c>
       <c r="AM19" t="n">
-        <v>0.75</v>
+        <v>0.001140594482421875</v>
       </c>
       <c r="AN19" t="n">
-        <v>0.5</v>
+        <v>6.866455078125e-05</v>
       </c>
       <c r="AO19" t="n">
-        <v>0.25</v>
+        <v>1.9073486328125e-06</v>
       </c>
       <c r="AP19" t="n">
         <v>0</v>
@@ -6230,130 +6230,130 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0</v>
+        <v>-1.308673858642578</v>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>-5.630516052246094</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>3.114253997802734</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>8.805658340454102</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>-1.593376159667969</v>
       </c>
       <c r="F20" t="n">
-        <v>0</v>
+        <v>-3.202648162841797</v>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>-3.214736938476562</v>
       </c>
       <c r="H20" t="n">
-        <v>0</v>
+        <v>-10.47328090667725</v>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>7.222700119018555</v>
       </c>
       <c r="J20" t="n">
-        <v>0</v>
+        <v>21.73056125640869</v>
       </c>
       <c r="K20" t="n">
-        <v>0</v>
+        <v>-9.328041076660156</v>
       </c>
       <c r="L20" t="n">
-        <v>0</v>
+        <v>-24.80213928222656</v>
       </c>
       <c r="M20" t="n">
-        <v>0</v>
+        <v>11.86023712158203</v>
       </c>
       <c r="N20" t="n">
-        <v>0</v>
+        <v>27.64601039886475</v>
       </c>
       <c r="O20" t="n">
-        <v>0</v>
+        <v>-8.769960403442383</v>
       </c>
       <c r="P20" t="n">
-        <v>0</v>
+        <v>-29.50358200073242</v>
       </c>
       <c r="Q20" t="n">
-        <v>0</v>
+        <v>-4.604013442993164</v>
       </c>
       <c r="R20" t="n">
-        <v>0</v>
+        <v>16.47088718414307</v>
       </c>
       <c r="S20" t="n">
-        <v>0</v>
+        <v>13.50650024414062</v>
       </c>
       <c r="T20" t="n">
-        <v>0.25</v>
+        <v>4.211666107177734</v>
       </c>
       <c r="U20" t="n">
-        <v>0.5</v>
+        <v>-10.59281158447266</v>
       </c>
       <c r="V20" t="n">
-        <v>0.75</v>
+        <v>-15.59666061401367</v>
       </c>
       <c r="W20" t="n">
-        <v>1</v>
+        <v>4.235427856445312</v>
       </c>
       <c r="X20" t="n">
-        <v>1.25</v>
+        <v>14.7276782989502</v>
       </c>
       <c r="Y20" t="n">
-        <v>1.5</v>
+        <v>-2.639408111572266</v>
       </c>
       <c r="Z20" t="n">
-        <v>1.75</v>
+        <v>-10.12635612487793</v>
       </c>
       <c r="AA20" t="n">
-        <v>2</v>
+        <v>7.66864013671875</v>
       </c>
       <c r="AB20" t="n">
-        <v>2.25</v>
+        <v>18.07172584533691</v>
       </c>
       <c r="AC20" t="n">
-        <v>2.5</v>
+        <v>6.323787689208984</v>
       </c>
       <c r="AD20" t="n">
-        <v>2.75</v>
+        <v>-6.142004013061523</v>
       </c>
       <c r="AE20" t="n">
-        <v>3</v>
+        <v>-4.418197631835938</v>
       </c>
       <c r="AF20" t="n">
-        <v>2.75</v>
+        <v>3.636054992675781</v>
       </c>
       <c r="AG20" t="n">
-        <v>2.5</v>
+        <v>7.350296020507812</v>
       </c>
       <c r="AH20" t="n">
-        <v>2.25</v>
+        <v>5.805862426757812</v>
       </c>
       <c r="AI20" t="n">
-        <v>2</v>
+        <v>2.913330078125</v>
       </c>
       <c r="AJ20" t="n">
-        <v>1.75</v>
+        <v>1.032260894775391</v>
       </c>
       <c r="AK20" t="n">
-        <v>1.5</v>
+        <v>0.2671279907226562</v>
       </c>
       <c r="AL20" t="n">
-        <v>1.25</v>
+        <v>0.05062484741210938</v>
       </c>
       <c r="AM20" t="n">
-        <v>1</v>
+        <v>0.0068817138671875</v>
       </c>
       <c r="AN20" t="n">
-        <v>0.75</v>
+        <v>0.0006380081176757812</v>
       </c>
       <c r="AO20" t="n">
-        <v>0.5</v>
+        <v>3.62396240234375e-05</v>
       </c>
       <c r="AP20" t="n">
-        <v>0.25</v>
+        <v>9.5367431640625e-07</v>
       </c>
       <c r="AQ20" t="n">
         <v>0</v>
@@ -6535,133 +6535,133 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0</v>
+        <v>1.506584167480469</v>
       </c>
       <c r="B21" t="n">
-        <v>0</v>
+        <v>-7.84197998046875</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>-4.103833198547363</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>11.15947341918945</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>4.41077709197998</v>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v>-2.3919677734375</v>
       </c>
       <c r="G21" t="n">
-        <v>0</v>
+        <v>0.4205794334411621</v>
       </c>
       <c r="H21" t="n">
-        <v>0</v>
+        <v>-15.6919994354248</v>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>-8.879220962524414</v>
       </c>
       <c r="J21" t="n">
-        <v>0</v>
+        <v>30.00593185424805</v>
       </c>
       <c r="K21" t="n">
-        <v>0</v>
+        <v>13.93830919265747</v>
       </c>
       <c r="L21" t="n">
-        <v>0</v>
+        <v>-35.39627838134766</v>
       </c>
       <c r="M21" t="n">
-        <v>0</v>
+        <v>-14.36383771896362</v>
       </c>
       <c r="N21" t="n">
-        <v>0</v>
+        <v>37.96110916137695</v>
       </c>
       <c r="O21" t="n">
-        <v>0</v>
+        <v>19.8048357963562</v>
       </c>
       <c r="P21" t="n">
-        <v>0</v>
+        <v>-31.58655548095703</v>
       </c>
       <c r="Q21" t="n">
-        <v>0</v>
+        <v>-27.59124803543091</v>
       </c>
       <c r="R21" t="n">
-        <v>0</v>
+        <v>7.415630340576172</v>
       </c>
       <c r="S21" t="n">
-        <v>0</v>
+        <v>19.63611078262329</v>
       </c>
       <c r="T21" t="n">
-        <v>0</v>
+        <v>16.26132202148438</v>
       </c>
       <c r="U21" t="n">
-        <v>0.25</v>
+        <v>-0.6886482238769531</v>
       </c>
       <c r="V21" t="n">
-        <v>0.5</v>
+        <v>-23.01078033447266</v>
       </c>
       <c r="W21" t="n">
-        <v>0.75</v>
+        <v>-10.92674160003662</v>
       </c>
       <c r="X21" t="n">
-        <v>1</v>
+        <v>18.16509628295898</v>
       </c>
       <c r="Y21" t="n">
-        <v>1.25</v>
+        <v>9.787609100341797</v>
       </c>
       <c r="Z21" t="n">
-        <v>1.5</v>
+        <v>-15.28038024902344</v>
       </c>
       <c r="AA21" t="n">
-        <v>1.75</v>
+        <v>-6.430400848388672</v>
       </c>
       <c r="AB21" t="n">
-        <v>2</v>
+        <v>18.7441520690918</v>
       </c>
       <c r="AC21" t="n">
-        <v>2.25</v>
+        <v>18.4306526184082</v>
       </c>
       <c r="AD21" t="n">
-        <v>2.5</v>
+        <v>-0.7710113525390625</v>
       </c>
       <c r="AE21" t="n">
-        <v>2.75</v>
+        <v>-9.30722713470459</v>
       </c>
       <c r="AF21" t="n">
-        <v>3</v>
+        <v>-2.248191833496094</v>
       </c>
       <c r="AG21" t="n">
-        <v>2.75</v>
+        <v>6.265392303466797</v>
       </c>
       <c r="AH21" t="n">
-        <v>2.5</v>
+        <v>8.024345397949219</v>
       </c>
       <c r="AI21" t="n">
-        <v>2.25</v>
+        <v>5.300130844116211</v>
       </c>
       <c r="AJ21" t="n">
-        <v>2</v>
+        <v>2.355361938476562</v>
       </c>
       <c r="AK21" t="n">
-        <v>1.75</v>
+        <v>0.7579460144042969</v>
       </c>
       <c r="AL21" t="n">
-        <v>1.5</v>
+        <v>0.1807479858398438</v>
       </c>
       <c r="AM21" t="n">
-        <v>1.25</v>
+        <v>0.0318751335144043</v>
       </c>
       <c r="AN21" t="n">
-        <v>1</v>
+        <v>0.004060745239257812</v>
       </c>
       <c r="AO21" t="n">
-        <v>0.75</v>
+        <v>0.000354766845703125</v>
       </c>
       <c r="AP21" t="n">
-        <v>0.5</v>
+        <v>1.9073486328125e-05</v>
       </c>
       <c r="AQ21" t="n">
-        <v>0.25</v>
+        <v>4.76837158203125e-07</v>
       </c>
       <c r="AR21" t="n">
         <v>0</v>
@@ -6840,136 +6840,136 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0</v>
+        <v>5.427574157714844</v>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>-5.036771297454834</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>-13.60455989837646</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>6.902168273925781</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>11.18649768829346</v>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
+        <v>-0.3968689441680908</v>
       </c>
       <c r="G22" t="n">
-        <v>0</v>
+        <v>7.070595264434814</v>
       </c>
       <c r="H22" t="n">
-        <v>0</v>
+        <v>-11.04209923744202</v>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>-31.72818660736084</v>
       </c>
       <c r="J22" t="n">
-        <v>0</v>
+        <v>18.5971667766571</v>
       </c>
       <c r="K22" t="n">
-        <v>0</v>
+        <v>46.63941431045532</v>
       </c>
       <c r="L22" t="n">
-        <v>0</v>
+        <v>-21.24520492553711</v>
       </c>
       <c r="M22" t="n">
-        <v>0</v>
+        <v>-51.04253149032593</v>
       </c>
       <c r="N22" t="n">
-        <v>0</v>
+        <v>20.87677240371704</v>
       </c>
       <c r="O22" t="n">
-        <v>0</v>
+        <v>54.57866811752319</v>
       </c>
       <c r="P22" t="n">
-        <v>0</v>
+        <v>-7.888513565063477</v>
       </c>
       <c r="Q22" t="n">
-        <v>0</v>
+        <v>-47.09234094619751</v>
       </c>
       <c r="R22" t="n">
-        <v>0</v>
+        <v>-16.19804906845093</v>
       </c>
       <c r="S22" t="n">
-        <v>0</v>
+        <v>15.21326494216919</v>
       </c>
       <c r="T22" t="n">
-        <v>0</v>
+        <v>26.4237015247345</v>
       </c>
       <c r="U22" t="n">
-        <v>0</v>
+        <v>18.94740295410156</v>
       </c>
       <c r="V22" t="n">
-        <v>0.25</v>
+        <v>-17.89173364639282</v>
       </c>
       <c r="W22" t="n">
-        <v>0.5</v>
+        <v>-31.51467990875244</v>
       </c>
       <c r="X22" t="n">
-        <v>0.75</v>
+        <v>7.807920932769775</v>
       </c>
       <c r="Y22" t="n">
-        <v>1</v>
+        <v>26.51034736633301</v>
       </c>
       <c r="Z22" t="n">
-        <v>1.25</v>
+        <v>-7.171375274658203</v>
       </c>
       <c r="AA22" t="n">
-        <v>1.5</v>
+        <v>-23.44266700744629</v>
       </c>
       <c r="AB22" t="n">
-        <v>1.75</v>
+        <v>6.313625335693359</v>
       </c>
       <c r="AC22" t="n">
-        <v>2</v>
+        <v>28.18823432922363</v>
       </c>
       <c r="AD22" t="n">
-        <v>2.25</v>
+        <v>13.09792852401733</v>
       </c>
       <c r="AE22" t="n">
-        <v>2.5</v>
+        <v>-8.568636894226074</v>
       </c>
       <c r="AF22" t="n">
-        <v>2.75</v>
+        <v>-10.03450155258179</v>
       </c>
       <c r="AG22" t="n">
-        <v>3</v>
+        <v>1.129123687744141</v>
       </c>
       <c r="AH22" t="n">
-        <v>2.75</v>
+        <v>8.506976127624512</v>
       </c>
       <c r="AI22" t="n">
-        <v>2.5</v>
+        <v>8.134622573852539</v>
       </c>
       <c r="AJ22" t="n">
-        <v>2.25</v>
+        <v>4.62645435333252</v>
       </c>
       <c r="AK22" t="n">
-        <v>2</v>
+        <v>1.845252990722656</v>
       </c>
       <c r="AL22" t="n">
-        <v>1.75</v>
+        <v>0.54378342628479</v>
       </c>
       <c r="AM22" t="n">
-        <v>1.5</v>
+        <v>0.1202187538146973</v>
       </c>
       <c r="AN22" t="n">
-        <v>1.25</v>
+        <v>0.0198209285736084</v>
       </c>
       <c r="AO22" t="n">
-        <v>1</v>
+        <v>0.002375602722167969</v>
       </c>
       <c r="AP22" t="n">
-        <v>0.75</v>
+        <v>0.0001962184906005859</v>
       </c>
       <c r="AQ22" t="n">
-        <v>0.5</v>
+        <v>1.001358032226562e-05</v>
       </c>
       <c r="AR22" t="n">
-        <v>0.25</v>
+        <v>2.384185791015625e-07</v>
       </c>
       <c r="AS22" t="n">
         <v>0</v>
@@ -7145,139 +7145,139 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0</v>
+        <v>7.945959806442261</v>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
+        <v>4.47929573059082</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>-19.57402968406677</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>-5.49336051940918</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>14.83601629734039</v>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>1.66108226776123</v>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>12.39321041107178</v>
       </c>
       <c r="H23" t="n">
-        <v>0</v>
+        <v>8.357291698455811</v>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>-46.5478196144104</v>
       </c>
       <c r="J23" t="n">
-        <v>0</v>
+        <v>-20.58663368225098</v>
       </c>
       <c r="K23" t="n">
-        <v>0</v>
+        <v>66.56060016155243</v>
       </c>
       <c r="L23" t="n">
-        <v>0</v>
+        <v>27.59576797485352</v>
       </c>
       <c r="M23" t="n">
-        <v>0</v>
+        <v>-72.103520154953</v>
       </c>
       <c r="N23" t="n">
-        <v>0</v>
+        <v>-31.93382740020752</v>
       </c>
       <c r="O23" t="n">
-        <v>0</v>
+        <v>68.96131110191345</v>
       </c>
       <c r="P23" t="n">
-        <v>0</v>
+        <v>42.94699096679688</v>
       </c>
       <c r="Q23" t="n">
-        <v>0</v>
+        <v>-42.93757319450378</v>
       </c>
       <c r="R23" t="n">
-        <v>0</v>
+        <v>-47.35085201263428</v>
       </c>
       <c r="S23" t="n">
-        <v>0</v>
+        <v>-6.097610354423523</v>
       </c>
       <c r="T23" t="n">
-        <v>0</v>
+        <v>24.55663251876831</v>
       </c>
       <c r="U23" t="n">
-        <v>0</v>
+        <v>41.10512053966522</v>
       </c>
       <c r="V23" t="n">
-        <v>0</v>
+        <v>7.33930778503418</v>
       </c>
       <c r="W23" t="n">
-        <v>0.25</v>
+        <v>-44.36450719833374</v>
       </c>
       <c r="X23" t="n">
-        <v>0.5</v>
+        <v>-21.20459270477295</v>
       </c>
       <c r="Y23" t="n">
-        <v>0.75</v>
+        <v>33.999995470047</v>
       </c>
       <c r="Z23" t="n">
-        <v>1</v>
+        <v>17.80513191223145</v>
       </c>
       <c r="AA23" t="n">
-        <v>1.25</v>
+        <v>-30.18516731262207</v>
       </c>
       <c r="AB23" t="n">
-        <v>1.5</v>
+        <v>-19.5018253326416</v>
       </c>
       <c r="AC23" t="n">
-        <v>1.75</v>
+        <v>24.79608273506165</v>
       </c>
       <c r="AD23" t="n">
-        <v>2</v>
+        <v>31.47636413574219</v>
       </c>
       <c r="AE23" t="n">
-        <v>2.25</v>
+        <v>2.997578144073486</v>
       </c>
       <c r="AF23" t="n">
-        <v>2.5</v>
+        <v>-14.88338184356689</v>
       </c>
       <c r="AG23" t="n">
-        <v>2.75</v>
+        <v>-8.141615152359009</v>
       </c>
       <c r="AH23" t="n">
-        <v>3</v>
+        <v>5.004226684570312</v>
       </c>
       <c r="AI23" t="n">
-        <v>2.75</v>
+        <v>10.07488346099854</v>
       </c>
       <c r="AJ23" t="n">
-        <v>2.5</v>
+        <v>7.771139144897461</v>
       </c>
       <c r="AK23" t="n">
-        <v>2.25</v>
+        <v>3.886588454246521</v>
       </c>
       <c r="AL23" t="n">
-        <v>2</v>
+        <v>1.40630054473877</v>
       </c>
       <c r="AM23" t="n">
-        <v>1.75</v>
+        <v>0.3822000026702881</v>
       </c>
       <c r="AN23" t="n">
-        <v>1.5</v>
+        <v>0.07874250411987305</v>
       </c>
       <c r="AO23" t="n">
-        <v>1.25</v>
+        <v>0.01218795776367188</v>
       </c>
       <c r="AP23" t="n">
-        <v>1</v>
+        <v>0.001379013061523438</v>
       </c>
       <c r="AQ23" t="n">
-        <v>0.75</v>
+        <v>0.0001080036163330078</v>
       </c>
       <c r="AR23" t="n">
-        <v>0.5</v>
+        <v>5.245208740234375e-06</v>
       </c>
       <c r="AS23" t="n">
-        <v>0.25</v>
+        <v>1.192092895507812e-07</v>
       </c>
       <c r="AT23" t="n">
         <v>0</v>

</xml_diff>